<commit_message>
new list of excel templates fitting last versions
</commit_message>
<xml_diff>
--- a/inst/extdata/minimal_example_excel_template.xlsx
+++ b/inst/extdata/minimal_example_excel_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C67DF82C-2FF6-2840-9FED-8B00B2D4AC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{C67DF82C-2FF6-2840-9FED-8B00B2D4AC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF6C4F41-EC6A-0142-99FE-D9EB12107C5F}"/>
   <bookViews>
-    <workbookView xWindow="16300" yWindow="1420" windowWidth="28800" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="28800" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -268,19 +268,19 @@
     <t>RNAPII</t>
   </si>
   <si>
-    <t>http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_3pseq/</t>
-  </si>
-  <si>
-    <t>http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_TTseq/</t>
-  </si>
-  <si>
-    <t>http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_RNAseq/</t>
-  </si>
-  <si>
-    <t>http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_ChIPseq/</t>
-  </si>
-  <si>
     <t>+PAP</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_TTseq/</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_RNAseq/</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_ChIPseq/</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_3pseq/</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +752,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I22" t="s">
         <v>37</v>
@@ -1701,10 +1701,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F3FB9481-5075-BD43-8802-C470E1B73EA6}"/>
-    <hyperlink ref="C42" r:id="rId2" xr:uid="{B71FE05B-4E94-204C-8212-126A2EC25BF0}"/>
-    <hyperlink ref="C50" r:id="rId3" xr:uid="{CE081A57-03EB-8545-9FF6-ED515FC84E88}"/>
-    <hyperlink ref="C58" r:id="rId4" xr:uid="{789F8E65-1649-D945-A802-9480409ED443}"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_3pseq/" xr:uid="{F3FB9481-5075-BD43-8802-C470E1B73EA6}"/>
+    <hyperlink ref="C42" r:id="rId2" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_TTseq/" xr:uid="{B71FE05B-4E94-204C-8212-126A2EC25BF0}"/>
+    <hyperlink ref="C50" r:id="rId3" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_RNAseq/" xr:uid="{CE081A57-03EB-8545-9FF6-ED515FC84E88}"/>
+    <hyperlink ref="C58" r:id="rId4" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_ChIPseq/" xr:uid="{789F8E65-1649-D945-A802-9480409ED443}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
batch removed from DATASET_OPTIONS in exported sNdR sample file
annotations with repeated disjoint feature names can be handled

change of several variable names
</commit_message>
<xml_diff>
--- a/inst/extdata/minimal_example_excel_template.xlsx
+++ b/inst/extdata/minimal_example_excel_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au103725/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B98E9A7-3419-624B-950A-F0CB06784843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{7B98E9A7-3419-624B-950A-F0CB06784843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50C241C3-11DC-904A-B260-76078ED66CE0}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="34080" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="1300" windowWidth="23940" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLES" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_3pseq/</t>
   </si>
   <si>
-    <t>siGFP_xPAP_in_batch1_plus.bw</t>
-  </si>
-  <si>
     <t>plus</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>GSM2642508_WIGfs_Hela-H9_WT_siFFL_Pol_II_N20_MA736_bin50_Scaled_BGSub_Hg38.bw</t>
+  </si>
+  <si>
+    <t>WT_1_EPAP_dedup_unique_tailed_Afilt_minus.bw</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -580,19 +582,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -600,10 +602,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -614,10 +616,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -628,10 +630,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -642,10 +644,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -656,10 +658,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -667,30 +669,30 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -698,13 +700,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -712,13 +714,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -726,13 +728,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -740,13 +742,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -757,22 +759,22 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -780,10 +782,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -794,10 +796,10 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -808,10 +810,10 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -819,30 +821,30 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -850,13 +852,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -864,13 +866,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -881,22 +883,22 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -904,10 +906,10 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -918,10 +920,10 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -932,10 +934,10 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -943,30 +945,30 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -974,13 +976,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -988,13 +990,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -1002,33 +1004,33 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
         <v>45</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>46</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
         <v>47</v>
       </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>48</v>
-      </c>
-      <c r="G30" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>